<commit_message>
Gestion stage adi et cir
</commit_message>
<xml_diff>
--- a/BobPlanning.back/files/EdtMacro.xlsx
+++ b/BobPlanning.back/files/EdtMacro.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="78">
   <si>
     <t>Numéro de la semaine</t>
   </si>
@@ -40,6 +40,9 @@
     <t>ADI1</t>
   </si>
   <si>
+    <t>ADI2</t>
+  </si>
+  <si>
     <t>AP5</t>
   </si>
   <si>
@@ -194,6 +197,12 @@
   </si>
   <si>
     <t>02/06/2025</t>
+  </si>
+  <si>
+    <t>Stage Exécutant 1 mois</t>
+  </si>
+  <si>
+    <t>Stage International Break 2 mois</t>
   </si>
   <si>
     <t>09/06/2025</t>
@@ -254,12 +263,17 @@
       <color rgb="FF0000"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF99"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -274,8 +288,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -616,42 +636,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:K55"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="11" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" ht="50" customHeight="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -659,25 +682,25 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -685,25 +708,25 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -711,25 +734,25 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -737,25 +760,25 @@
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -763,25 +786,25 @@
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -789,25 +812,25 @@
         <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -815,25 +838,25 @@
         <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -841,25 +864,25 @@
         <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -867,25 +890,25 @@
         <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -893,54 +916,57 @@
         <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I12" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="J12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -948,25 +974,25 @@
         <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -974,25 +1000,25 @@
         <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1000,25 +1026,25 @@
         <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1026,25 +1052,25 @@
         <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1052,25 +1078,25 @@
         <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1078,25 +1104,25 @@
         <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1104,83 +1130,89 @@
         <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="J20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
         <v>34</v>
       </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" t="s">
-        <v>33</v>
-      </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I21" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="J21" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1188,25 +1220,25 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1214,25 +1246,25 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1240,25 +1272,25 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1266,25 +1298,25 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1292,25 +1324,25 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1318,25 +1350,25 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1344,83 +1376,89 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="J29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>10</v>
       </c>
       <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
         <v>44</v>
       </c>
-      <c r="C30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" t="s">
-        <v>43</v>
-      </c>
       <c r="F30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I30" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="J30" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1428,25 +1466,25 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1454,25 +1492,25 @@
         <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1480,25 +1518,25 @@
         <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1506,25 +1544,25 @@
         <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1532,25 +1570,25 @@
         <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1558,83 +1596,89 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H36" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="J37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>18</v>
       </c>
       <c r="B38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s">
         <v>53</v>
       </c>
-      <c r="C38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" t="s">
-        <v>52</v>
-      </c>
       <c r="F38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I38" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="J38" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1642,25 +1686,25 @@
         <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>55</v>
+        <v>12</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="F39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1668,25 +1712,25 @@
         <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1694,25 +1738,25 @@
         <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1720,387 +1764,441 @@
         <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>59</v>
+        <v>12</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="F42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H42" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>23</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H43" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="I43" t="s">
+        <v>62</v>
+      </c>
+      <c r="J43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>24</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F44" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" t="s">
         <v>62</v>
       </c>
-      <c r="F44" t="s">
-        <v>11</v>
-      </c>
-      <c r="G44" t="s">
-        <v>11</v>
-      </c>
-      <c r="H44" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>25</v>
       </c>
       <c r="B45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" t="s">
+        <v>62</v>
+      </c>
+      <c r="J45" t="s">
         <v>63</v>
       </c>
-      <c r="C45" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" t="s">
-        <v>11</v>
-      </c>
-      <c r="F45" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" t="s">
-        <v>11</v>
-      </c>
-      <c r="H45" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>26</v>
       </c>
       <c r="B46" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H46" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="I46" t="s">
+        <v>62</v>
+      </c>
+      <c r="J46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>27</v>
       </c>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H47" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="I47" t="s">
+        <v>62</v>
+      </c>
+      <c r="J47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>28</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I48" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="J48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>29</v>
       </c>
       <c r="B49" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E49" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I49" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="J49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>30</v>
       </c>
       <c r="B50" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I50" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="J50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>31</v>
       </c>
       <c r="B51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" t="s">
         <v>70</v>
       </c>
-      <c r="C51" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" t="s">
-        <v>67</v>
-      </c>
       <c r="F51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I51" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="J51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>32</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E52" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I52" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="J52" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>33</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E53" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I53" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="J53" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>34</v>
       </c>
       <c r="B54" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E54" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I54" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="J54" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D55" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E55" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F55" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G55" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H55" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I55" t="s">
-        <v>23</v>
+        <v>62</v>
+      </c>
+      <c r="J55" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>